<commit_message>
edit add course with co-instructor
</commit_message>
<xml_diff>
--- a/frontend/src/Example.xlsx
+++ b/frontend/src/Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nomon\OneDrive\Desktop\cmu-score-announcement\frontend\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EC5F1A-9B37-41CD-BF3D-8723065EE669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0500227A-BC7F-4214-9FCD-DE6AB7FD2D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5E4923E5-E3E3-45FB-AEBA-DD38CD184FF4}"/>
+    <workbookView xWindow="8232" yWindow="108" windowWidth="11556" windowHeight="12852" xr2:uid="{5E4923E5-E3E3-45FB-AEBA-DD38CD184FF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -665,7 +665,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -752,6 +752,9 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
@@ -772,6 +775,9 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
@@ -792,7 +798,9 @@
       </c>
     </row>
     <row r="6" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
+      <c r="A6" s="5">
+        <v>1</v>
+      </c>
       <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
@@ -836,6 +844,9 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
@@ -856,6 +867,9 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
@@ -876,6 +890,9 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>2</v>
+      </c>
       <c r="B10" s="2" t="s">
         <v>22</v>
       </c>

</xml_diff>